<commit_message>
Add holdings module to calculate historical balances and integrate into accounts.
</commit_message>
<xml_diff>
--- a/data/demo_data.xlsx
+++ b/data/demo_data.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Projects\personal-finance\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2291ECAA-A8C1-42C3-98B2-4BB3CAF5513E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C1FF53-72AB-40F9-BCC9-89AEC6678BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Accounts" sheetId="13" r:id="rId1"/>
-    <sheet name="Barclays" sheetId="1" r:id="rId2"/>
-    <sheet name="Santander" sheetId="17" r:id="rId3"/>
-    <sheet name="AMEX" sheetId="21" r:id="rId4"/>
-    <sheet name="Chase - Saver" sheetId="20" r:id="rId5"/>
-    <sheet name="Revolut - Savings" sheetId="19" r:id="rId6"/>
-    <sheet name="Revolut" sheetId="18" r:id="rId7"/>
+    <sheet name="Holdings" sheetId="22" r:id="rId2"/>
+    <sheet name="Barclays" sheetId="1" r:id="rId3"/>
+    <sheet name="Santander" sheetId="17" r:id="rId4"/>
+    <sheet name="AMEX" sheetId="21" r:id="rId5"/>
+    <sheet name="Chase - Saver" sheetId="20" r:id="rId6"/>
+    <sheet name="Revolut - Savings" sheetId="19" r:id="rId7"/>
+    <sheet name="Revolut" sheetId="18" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -108,6 +109,39 @@
   </si>
   <si>
     <t>Chase - Saver</t>
+  </si>
+  <si>
+    <t>Full name</t>
+  </si>
+  <si>
+    <t>ISIN</t>
+  </si>
+  <si>
+    <t>YF name</t>
+  </si>
+  <si>
+    <t>Transaction type</t>
+  </si>
+  <si>
+    <t>Shares</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>Buy</t>
+  </si>
+  <si>
+    <t>Fidelity Index World Fund</t>
+  </si>
+  <si>
+    <t>GB00BJS8SJ34</t>
+  </si>
+  <si>
+    <t>0P000125KV.L</t>
   </si>
 </sst>
 </file>
@@ -663,7 +697,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -681,13 +715,15 @@
     <xf numFmtId="8" fontId="18" fillId="33" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="18" fillId="33" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1012,12 +1048,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF82C24B-DC0D-42C3-92C2-5EDB4088032B}">
   <sheetPr>
-    <tabColor theme="1"/>
+    <tabColor theme="0"/>
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1175,6 +1211,87 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86529CC4-E09A-4EFF-BFDA-B5BFB94D7FAD}">
+  <sheetPr>
+    <tabColor theme="0"/>
+  </sheetPr>
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>45919</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2">
+        <v>981.10736799999995</v>
+      </c>
+      <c r="G2" s="11">
+        <f t="shared" ref="G2" si="0">H2/F2</f>
+        <v>3.9751001034170197</v>
+      </c>
+      <c r="H2" s="11">
+        <v>3900</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C227"/>
   <sheetViews>
@@ -3689,7 +3806,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A4EE4A-5640-46BD-A19F-1AAEC67D31FB}">
   <dimension ref="A1:C159"/>
   <sheetViews>
@@ -5457,7 +5574,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{320D7F72-4D95-4E6D-99D3-871A7B2A7B13}">
   <dimension ref="A1:C479"/>
   <sheetViews>
@@ -10745,7 +10862,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCDFB4AD-875B-4433-BD4D-F0C523601563}">
   <dimension ref="A1:C23"/>
   <sheetViews>
@@ -11038,7 +11155,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D065F088-6A52-4642-8576-8D3EA41B5804}">
   <dimension ref="A1:C23"/>
   <sheetViews>
@@ -11103,7 +11220,7 @@
         <v>45382</v>
       </c>
       <c r="B5" s="6">
-        <f t="shared" ref="B5:B23" si="1">B4+100</f>
+        <f t="shared" ref="B5" si="1">B4+100</f>
         <v>151</v>
       </c>
       <c r="C5" s="5">
@@ -11128,7 +11245,7 @@
         <v>45442</v>
       </c>
       <c r="B7" s="6">
-        <f t="shared" ref="B7:B23" si="2">B6+100</f>
+        <f t="shared" ref="B7" si="2">B6+100</f>
         <v>152</v>
       </c>
       <c r="C7" s="5">
@@ -11153,7 +11270,7 @@
         <v>45502</v>
       </c>
       <c r="B9" s="6">
-        <f t="shared" ref="B9:B23" si="3">B8+100</f>
+        <f t="shared" ref="B9" si="3">B8+100</f>
         <v>153</v>
       </c>
       <c r="C9" s="5">
@@ -11178,7 +11295,7 @@
         <v>45562</v>
       </c>
       <c r="B11" s="6">
-        <f t="shared" ref="B11:B23" si="4">B10+100</f>
+        <f t="shared" ref="B11" si="4">B10+100</f>
         <v>154</v>
       </c>
       <c r="C11" s="5">
@@ -11203,7 +11320,7 @@
         <v>45622</v>
       </c>
       <c r="B13" s="6">
-        <f t="shared" ref="B13:B23" si="5">B12+100</f>
+        <f t="shared" ref="B13" si="5">B12+100</f>
         <v>155</v>
       </c>
       <c r="C13" s="5">
@@ -11228,7 +11345,7 @@
         <v>45682</v>
       </c>
       <c r="B15" s="6">
-        <f t="shared" ref="B15:B23" si="6">B14+100</f>
+        <f t="shared" ref="B15" si="6">B14+100</f>
         <v>156</v>
       </c>
       <c r="C15" s="5">
@@ -11253,7 +11370,7 @@
         <v>45742</v>
       </c>
       <c r="B17" s="6">
-        <f t="shared" ref="B17:B23" si="7">B16+100</f>
+        <f t="shared" ref="B17" si="7">B16+100</f>
         <v>157</v>
       </c>
       <c r="C17" s="5">
@@ -11278,7 +11395,7 @@
         <v>45802</v>
       </c>
       <c r="B19" s="6">
-        <f t="shared" ref="B19:B23" si="8">B18+100</f>
+        <f t="shared" ref="B19" si="8">B18+100</f>
         <v>158</v>
       </c>
       <c r="C19" s="5">
@@ -11303,7 +11420,7 @@
         <v>45862</v>
       </c>
       <c r="B21" s="6">
-        <f t="shared" ref="B21:B23" si="9">B20+100</f>
+        <f t="shared" ref="B21" si="9">B20+100</f>
         <v>159</v>
       </c>
       <c r="C21" s="5">
@@ -11340,7 +11457,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A33F5135-72CE-41E2-AE52-06530DC25488}">
   <dimension ref="A1:C49"/>
   <sheetViews>

</xml_diff>